<commit_message>
add av folder content
</commit_message>
<xml_diff>
--- a/Android/framework/Basic_linux.xlsx
+++ b/Android/framework/Basic_linux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tree" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,8 +24,88 @@
 </workbook>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C76" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">权限接口</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C80" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">文件读写操作接口封装</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">DRM Info请求队列缓存</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L66" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">DRM info队列缓存</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L71" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">drm数据缓存队列</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7758" uniqueCount="4707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7873" uniqueCount="4800">
   <si>
     <t xml:space="preserve">.</t>
   </si>
@@ -14094,7 +14174,288 @@
     <t xml:space="preserve">tools</t>
   </si>
   <si>
+    <t xml:space="preserve">aidl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">camera2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cameraserver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tests</t>
+  </si>
+  <si>
     <t xml:space="preserve">Android系统中追加的命令行工具</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screenrecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stagefright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">功能:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生成静态库</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libdrmframeworkcommon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmEngineBase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDrmEngine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDrmManagerService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDrmServiceListener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReadWriteUtils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmConstraints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmConvertedStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmInfoEvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmInfoRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmInfoStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmMetadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmRights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrmSupportInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drmserver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libdrmframework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libmediadrm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediacas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediadrm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audioserver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android.mk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生成audioserver可执行程序</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audioserver.rc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启动audioserer可执行程序</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main_audioserver.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启动</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MediaLogService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">调用BinderService类中的instantiate函数将service追加到servicemanager中</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AudioFlinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AudioPolicyService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAudioService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoundTriggerHwService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生成共享库libcommon_time_client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc_helper.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">帮助通信类,在发生common time通信异常时,操作本类</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICommonClock.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IcommonClockListener/IcommonClock service定义</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICommonTimeConfig.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICommonTimeConfigservice定义</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local_clock.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">调用hardware/local_time_hal.h接口获取时间</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utils.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#include &lt;arpa/inet.h&gt;
+#include &lt;linux/socket.h&gt;
+#include &lt;binder/Parcel.h&gt;读取socker地址</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utils.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extractors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_utils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libaaudio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libaudioclient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libaudiohal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libaudioprocessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libcpustats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libeffects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libheif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libmedia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libmediaextractor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libmediametrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libmediaplayer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libmediaplayerservice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libnbaio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libnblog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libstagefright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediaserver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mtp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MediaComponents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">不参与编译</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audioflinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audiopolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediaanalytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediacodec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medialog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediaresourcemanager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minijail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oboeservice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISoundTriggerClient.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsoundTrigger.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IsoundTriggerHwService.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoundTriggerCallback.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SoundTrigger.h</t>
   </si>
   <si>
     <t xml:space="preserve">ps -A</t>
@@ -14152,10 +14513,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -14181,17 +14543,55 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6666FF"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -14298,7 +14698,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -14343,12 +14743,72 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -14360,6 +14820,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF6666FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3C3C3C"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -14374,9 +14894,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>513720</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>106</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14389,8 +14909,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="780840" y="498600"/>
-          <a:ext cx="11448360" cy="16909920"/>
+          <a:off x="771480" y="498600"/>
+          <a:ext cx="11314440" cy="16909560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14418,7 +14938,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="2.04639175257732"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="1.90721649484536"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -52995,12 +53515,12 @@
   <dimension ref="H3:U25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.1855670103093"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0463917525773"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -53241,7 +53761,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.1855670103093"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0463917525773"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -53269,175 +53789,1077 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:L43"/>
+  <dimension ref="A3:O282"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L144" activeCellId="0" sqref="L144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="11" width="11.319587628866"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16" t="s">
+        <v>4681</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>4682</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="I4" s="16" t="s">
+        <v>4683</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="L4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="15"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="15"/>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="15"/>
+      <c r="C8" s="16" t="s">
+        <v>4684</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>4685</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="I8" s="16" t="s">
+        <v>4686</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="15"/>
+      <c r="L10" s="17"/>
+    </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="4"/>
+      <c r="B11" s="15"/>
+      <c r="L11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16" t="s">
+        <v>4687</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="F12" s="16" t="s">
+        <v>4688</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="15"/>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="20"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="21" t="s">
         <v>4681</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="F12" s="11" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="11" t="s">
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="11" t="s">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="11" t="s">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11" t="s">
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="11" t="s">
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="21" t="s">
         <v>4682</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="I12" s="11" t="s">
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="11" t="s">
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="11" t="s">
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="11" t="s">
+        <v>4696</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="21" t="s">
         <v>4683</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5"/>
-      <c r="C16" s="11" t="s">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="22" t="s">
+        <v>4697</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13"/>
+      <c r="M53" s="13"/>
+      <c r="N53" s="14"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="15" t="s">
+        <v>4698</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>4699</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>4700</v>
+      </c>
+      <c r="N54" s="17"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="15"/>
+      <c r="N55" s="17"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="15"/>
+      <c r="C56" s="22" t="s">
+        <v>4701</v>
+      </c>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="14"/>
+      <c r="N56" s="17"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="23" t="s">
+        <v>4702</v>
+      </c>
+      <c r="E57" s="23"/>
+      <c r="G57" s="23" t="s">
+        <v>4703</v>
+      </c>
+      <c r="H57" s="23"/>
+      <c r="J57" s="24" t="s">
+        <v>4704</v>
+      </c>
+      <c r="K57" s="24"/>
+      <c r="L57" s="17"/>
+      <c r="N57" s="17"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="17"/>
+      <c r="N58" s="17"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="L59" s="17"/>
+      <c r="N59" s="17"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="23" t="s">
+        <v>4705</v>
+      </c>
+      <c r="E60" s="23"/>
+      <c r="G60" s="23" t="s">
+        <v>4706</v>
+      </c>
+      <c r="H60" s="23"/>
+      <c r="L60" s="17"/>
+      <c r="N60" s="17"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="L61" s="17"/>
+      <c r="N61" s="17"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="15"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="20"/>
+      <c r="N62" s="17"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="15"/>
+      <c r="N63" s="17"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="15"/>
+      <c r="N64" s="17"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="15"/>
+      <c r="N65" s="17"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="15"/>
+      <c r="C66" s="23" t="s">
+        <v>4707</v>
+      </c>
+      <c r="D66" s="23"/>
+      <c r="F66" s="23" t="s">
+        <v>4708</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="I66" s="23" t="s">
+        <v>4702</v>
+      </c>
+      <c r="J66" s="23"/>
+      <c r="L66" s="23" t="s">
+        <v>4709</v>
+      </c>
+      <c r="M66" s="23"/>
+      <c r="N66" s="17"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="15"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="23"/>
+      <c r="N67" s="17"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="15"/>
+      <c r="N68" s="17"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="15"/>
+      <c r="N69" s="17"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="15"/>
+      <c r="N70" s="17"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="15"/>
+      <c r="C71" s="23" t="s">
+        <v>4710</v>
+      </c>
+      <c r="D71" s="23"/>
+      <c r="F71" s="23" t="s">
+        <v>4711</v>
+      </c>
+      <c r="G71" s="23"/>
+      <c r="I71" s="23" t="s">
+        <v>4712</v>
+      </c>
+      <c r="J71" s="23"/>
+      <c r="L71" s="23" t="s">
+        <v>4713</v>
+      </c>
+      <c r="M71" s="23"/>
+      <c r="N71" s="17"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="15"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="23"/>
+      <c r="I72" s="23"/>
+      <c r="J72" s="23"/>
+      <c r="L72" s="23"/>
+      <c r="M72" s="23"/>
+      <c r="N72" s="17"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="15"/>
+      <c r="N73" s="17"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="15"/>
+      <c r="N74" s="17"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="15"/>
+      <c r="N75" s="17"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="15"/>
+      <c r="C76" s="23" t="s">
+        <v>4714</v>
+      </c>
+      <c r="D76" s="23"/>
+      <c r="F76" s="23" t="s">
+        <v>4715</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="I76" s="23" t="s">
+        <v>4704</v>
+      </c>
+      <c r="J76" s="23"/>
+      <c r="L76" s="23" t="s">
+        <v>4705</v>
+      </c>
+      <c r="M76" s="23"/>
+      <c r="N76" s="17"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="15"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="I77" s="23"/>
+      <c r="J77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="M77" s="23"/>
+      <c r="N77" s="17"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="15"/>
+      <c r="N78" s="17"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="15"/>
+      <c r="N79" s="17"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="15"/>
+      <c r="C80" s="23" t="s">
+        <v>4706</v>
+      </c>
+      <c r="D80" s="23"/>
+      <c r="N80" s="17"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="15"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="N81" s="17"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="15"/>
+      <c r="N82" s="17"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="18"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
+      <c r="J83" s="19"/>
+      <c r="K83" s="19"/>
+      <c r="L83" s="19"/>
+      <c r="M83" s="19"/>
+      <c r="N83" s="20"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="11" t="s">
+        <v>4716</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="11" t="s">
+        <v>4717</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="11" t="s">
+        <v>4718</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="11" t="s">
+        <v>4719</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="11" t="s">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="21" t="s">
         <v>4684</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="F16" s="11" t="s">
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+      <c r="J103" s="21"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="21"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="11" t="s">
+        <v>4721</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="11" t="s">
+        <v>4722</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C107" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>4723</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C109" s="11" t="s">
+        <v>4724</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>4725</v>
+      </c>
+      <c r="G110" s="25"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G111" s="25"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="11" t="s">
+        <v>4726</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C113" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>4727</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>4728</v>
+      </c>
+      <c r="F113" s="0"/>
+      <c r="H113" s="26" t="s">
+        <v>4729</v>
+      </c>
+      <c r="I113" s="26"/>
+      <c r="J113" s="26"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+      <c r="M113" s="26"/>
+      <c r="N113" s="26"/>
+      <c r="O113" s="26"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E114" s="11" t="s">
+        <v>4730</v>
+      </c>
+      <c r="F114" s="0"/>
+      <c r="H114" s="26"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="26"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+      <c r="M114" s="26"/>
+      <c r="N114" s="26"/>
+      <c r="O114" s="26"/>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E115" s="11" t="s">
+        <v>4731</v>
+      </c>
+      <c r="F115" s="0"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="26"/>
+      <c r="L115" s="26"/>
+      <c r="M115" s="26"/>
+      <c r="N115" s="26"/>
+      <c r="O115" s="26"/>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E116" s="11" t="s">
+        <v>4732</v>
+      </c>
+      <c r="F116" s="0"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="26"/>
+      <c r="K116" s="26"/>
+      <c r="L116" s="26"/>
+      <c r="M116" s="26"/>
+      <c r="N116" s="26"/>
+      <c r="O116" s="26"/>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E117" s="11" t="s">
+        <v>4733</v>
+      </c>
+      <c r="F117" s="0"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="26"/>
+      <c r="K117" s="26"/>
+      <c r="L117" s="26"/>
+      <c r="M117" s="26"/>
+      <c r="N117" s="26"/>
+      <c r="O117" s="26"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F118" s="0"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F119" s="0"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="11" t="s">
+        <v>4734</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="11" t="s">
+        <v>4722</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C123" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>4735</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C125" s="11" t="s">
+        <v>4736</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>4737</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="11" t="s">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>4739</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="11" t="s">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D132" s="11" t="s">
+        <v>4741</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="11" t="s">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D135" s="11" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C137" s="11" t="s">
+        <v>4744</v>
+      </c>
+      <c r="D137" s="27" t="s">
+        <v>4745</v>
+      </c>
+      <c r="E137" s="27"/>
+      <c r="F137" s="27"/>
+      <c r="G137" s="27"/>
+      <c r="H137" s="27"/>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="11" t="s">
+        <v>4746</v>
+      </c>
+      <c r="D138" s="27"/>
+      <c r="E138" s="27"/>
+      <c r="F138" s="27"/>
+      <c r="G138" s="27"/>
+      <c r="H138" s="27"/>
+    </row>
+    <row r="139" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="11" t="s">
+        <v>4698</v>
+      </c>
+      <c r="D139" s="27"/>
+      <c r="E139" s="27"/>
+      <c r="F139" s="27"/>
+      <c r="G139" s="27"/>
+      <c r="H139" s="27"/>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C140" s="0"/>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="0"/>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="11" t="s">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="11" t="s">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="11" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="11" t="s">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="11" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="11" t="s">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="11" t="s">
+        <v>4753</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B171" s="11" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="11" t="s">
+        <v>4755</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B176" s="11" t="s">
+        <v>4756</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B179" s="11" t="s">
+        <v>4757</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B181" s="11" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="11" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B185" s="11" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B187" s="11" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B189" s="11" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B191" s="11" t="s">
+        <v>4763</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B194" s="11" t="s">
+        <v>4764</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B196" s="11" t="s">
+        <v>4765</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B198" s="11" t="s">
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B200" s="11" t="s">
+        <v>4766</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="21" t="s">
         <v>4685</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="I16" s="11" t="s">
+      <c r="B207" s="21"/>
+      <c r="C207" s="21"/>
+      <c r="D207" s="21"/>
+      <c r="E207" s="21"/>
+      <c r="F207" s="21"/>
+      <c r="G207" s="21"/>
+      <c r="H207" s="21"/>
+      <c r="I207" s="21"/>
+      <c r="J207" s="21"/>
+      <c r="K207" s="21"/>
+      <c r="L207" s="21"/>
+      <c r="M207" s="21"/>
+    </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B208" s="11" t="s">
+        <v>4767</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B209" s="11" t="s">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="21" t="s">
         <v>4686</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5"/>
-      <c r="C20" s="11" t="s">
-        <v>4686</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="F20" s="11" t="s">
+      <c r="B216" s="21"/>
+      <c r="C216" s="21"/>
+      <c r="D216" s="21"/>
+      <c r="E216" s="21"/>
+      <c r="F216" s="21"/>
+      <c r="G216" s="21"/>
+      <c r="H216" s="21"/>
+      <c r="I216" s="21"/>
+      <c r="J216" s="21"/>
+      <c r="K216" s="21"/>
+      <c r="L216" s="21"/>
+      <c r="M216" s="21"/>
+    </row>
+    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B217" s="11" t="s">
+        <v>4769</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B221" s="11" t="s">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B228" s="11" t="s">
+        <v>4681</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B234" s="11" t="s">
+        <v>4771</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B239" s="11" t="s">
+        <v>4772</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B244" s="11" t="s">
+        <v>4720</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B249" s="11" t="s">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B254" s="11" t="s">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B259" s="11" t="s">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B264" s="11" t="s">
+        <v>4776</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B270" s="11" t="s">
         <v>4687</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="I20" s="11" t="s">
-        <v>4688</v>
-      </c>
-      <c r="J20" s="11"/>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5"/>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="10"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>4682</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>4689</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="s">
+    </row>
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="21" t="s">
         <v>4687</v>
       </c>
+      <c r="B276" s="21"/>
+      <c r="C276" s="21"/>
+      <c r="D276" s="21"/>
+      <c r="E276" s="21"/>
+      <c r="F276" s="21"/>
+      <c r="G276" s="21"/>
+      <c r="H276" s="21"/>
+      <c r="I276" s="21"/>
+      <c r="J276" s="21"/>
+      <c r="K276" s="21"/>
+      <c r="L276" s="21"/>
+      <c r="M276" s="21"/>
+    </row>
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B277" s="11" t="s">
+        <v>4777</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B278" s="11" t="s">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B279" s="11" t="s">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B280" s="11" t="s">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B281" s="11" t="s">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B282" s="11" t="s">
+        <v>4782</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="28">
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="F4:G5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="I8:J9"/>
     <mergeCell ref="C12:D13"/>
     <mergeCell ref="F12:G13"/>
-    <mergeCell ref="I12:J13"/>
-    <mergeCell ref="C16:D17"/>
-    <mergeCell ref="F16:G17"/>
-    <mergeCell ref="I16:J17"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="I20:J21"/>
+    <mergeCell ref="D57:E58"/>
+    <mergeCell ref="G57:H58"/>
+    <mergeCell ref="J57:K58"/>
+    <mergeCell ref="D60:E61"/>
+    <mergeCell ref="G60:H61"/>
+    <mergeCell ref="C66:D67"/>
+    <mergeCell ref="F66:G67"/>
+    <mergeCell ref="I66:J67"/>
+    <mergeCell ref="L66:M67"/>
+    <mergeCell ref="C71:D72"/>
+    <mergeCell ref="F71:G72"/>
+    <mergeCell ref="I71:J72"/>
+    <mergeCell ref="L71:M72"/>
+    <mergeCell ref="C76:D77"/>
+    <mergeCell ref="F76:G77"/>
+    <mergeCell ref="I76:J77"/>
+    <mergeCell ref="L76:M77"/>
+    <mergeCell ref="C80:D81"/>
+    <mergeCell ref="H113:O117"/>
+    <mergeCell ref="D137:H139"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -53446,6 +54868,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -53456,91 +54879,91 @@
   </sheetPr>
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4587628865979"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7319587628866"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.319587628866"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5927835051546"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.319587628866"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>4690</v>
+        <v>4783</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4691</v>
+        <v>4784</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>4692</v>
+        <v>4785</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4693</v>
+        <v>4786</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>4694</v>
+        <v>4787</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>4695</v>
+        <v>4788</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>4696</v>
+        <v>4789</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>4697</v>
+        <v>4790</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>4698</v>
+        <v>4791</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>4699</v>
+        <v>4792</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>4700</v>
+        <v>4793</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>4701</v>
+        <v>4794</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>4702</v>
+        <v>4795</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>4703</v>
+        <v>4796</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>4704</v>
+        <v>4797</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>4705</v>
+        <v>4798</v>
       </c>
     </row>
   </sheetData>
@@ -53567,12 +54990,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.319587628866"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>4706</v>
+        <v>4799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>